<commit_message>
some graphs in report
</commit_message>
<xml_diff>
--- a/cw/reportfiles/reportready-alpha-10h1000epo.xlsx
+++ b/cw/reportfiles/reportready-alpha-10h1000epo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ardadogan/Documents/code/AI/semester2/cw/reportfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581C3F0E-48A6-6E40-9A77-96283963A5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE411D9-4D72-3D46-8110-D213341CE6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -604,7 +604,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Effect of alpha value on MSE</a:t>
+              <a:t>Effect of alpha value on MSE (10 hidden nodes, 1000</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> epochs)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
             </a:r>
           </a:p>
         </c:rich>

</xml_diff>